<commit_message>
MongoDB data now being rendered to dashboard.
</commit_message>
<xml_diff>
--- a/spurs/test_spurs_data.xlsx
+++ b/spurs/test_spurs_data.xlsx
@@ -17,12 +17,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Player Display Name</t>
-  </si>
-  <si>
-    <t>Session Date</t>
-  </si>
   <si>
     <t>Dynamic Stress Load</t>
   </si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>Holtby</t>
+  </si>
+  <si>
+    <t>Player_Display_Name</t>
+  </si>
+  <si>
+    <t>Session_Date</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:E4446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,24 +456,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>41837</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>41837</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>41837</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>41837</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>41837</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>41837</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>41837</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>41837</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>41837</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>41837</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <v>41837</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>41837</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
         <v>41837</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>41837</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>41837</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>41837</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>41837</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
         <v>41837</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
         <v>41837</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2">
         <v>41837</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2">
         <v>41837</v>

</xml_diff>

<commit_message>
Basic client side routing now rendering DB data to html.
</commit_message>
<xml_diff>
--- a/spurs/test_spurs_data.xlsx
+++ b/spurs/test_spurs_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Dynamic Stress Load</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Session_Date</t>
+  </si>
+  <si>
+    <t>Ronaldo</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:E4446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>41837</v>
+        <v>41838</v>
       </c>
       <c r="C2" s="3">
         <v>216.17</v>
@@ -829,25 +832,55 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>41838</v>
+      </c>
+      <c r="C23" s="3">
+        <v>216.17</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.78848379629629628</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.85276620370370371</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>41838</v>
+      </c>
+      <c r="C24" s="3">
+        <v>246</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.78848379629629628</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.85276620370370371</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
+        <v>41839</v>
+      </c>
+      <c r="C25" s="3">
+        <v>246</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.78848379629629628</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.85276620370370371</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>

</xml_diff>